<commit_message>
Replace PI with PID
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_olpi.xlsx
+++ b/andes/cases/ieee14/ieee14_olpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD85BBE0-E3F9-A749-8E2D-F218266C06C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862AFBF0-0000-2146-855B-6292B5AAE103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36220" yWindow="-2240" windowWidth="34560" windowHeight="19440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="177">
   <si>
     <t>uid</t>
   </si>
@@ -559,6 +559,12 @@
   </si>
   <si>
     <t>gov</t>
+  </si>
+  <si>
+    <t>kD</t>
+  </si>
+  <si>
+    <t>tD</t>
   </si>
 </sst>
 </file>
@@ -1031,15 +1037,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96458FAA-7322-424B-9E72-5787496A0A03}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1055,8 +1061,14 @@
       <c r="E1" s="4" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1067,10 +1079,16 @@
         <v>130</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5180,7 +5198,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change PID input from pout to wd
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_olpi.xlsx
+++ b/andes/cases/ieee14/ieee14_olpi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{862AFBF0-0000-2146-855B-6292B5AAE103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004EE4FC-9FEE-DE46-B297-2892F62D3A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36220" yWindow="-2240" windowWidth="34560" windowHeight="19440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1079,10 +1079,10 @@
         <v>130</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>

<commit_message>
Add case for olpi
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/ieee14_olpi.xlsx
+++ b/andes/cases/ieee14/ieee14_olpi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jinningwang/Documents/work/andes/andes/cases/ieee14/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004EE4FC-9FEE-DE46-B297-2892F62D3A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1759BAAE-90C8-1D40-9F76-EDE9B89B0774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36220" yWindow="-2240" windowWidth="34560" windowHeight="19440" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-3600" windowWidth="19200" windowHeight="21600" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Toggler" sheetId="1" r:id="rId1"/>
@@ -1040,7 +1040,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1082,7 @@
         <v>0.05</v>
       </c>
       <c r="E2">
-        <v>0.01</v>
+        <v>0.1</v>
       </c>
       <c r="F2">
         <v>0</v>

</xml_diff>